<commit_message>
a lot (login + register)
</commit_message>
<xml_diff>
--- a/life pulse clinic/accountsTable.xlsx
+++ b/life pulse clinic/accountsTable.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hala_\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hala_\Documents\GitHub\life-pulse-clinic\life pulse clinic\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{725FEB7F-48A2-481D-A257-3D7A50E101B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6827AA23-8C29-4751-8ACB-7A5066DF5EDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4728657F-F0D8-498A-B068-B8A7D909C1FB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{CA59212C-BBDD-4EF6-9806-A4551CD527C4}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="גיליון1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,25 +35,36 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t>Username</t>
+    <t>malakggh</t>
   </si>
   <si>
-    <t>Password</t>
+    <t>hayaab</t>
   </si>
   <si>
-    <t>malakggh</t>
+    <t>123456a$</t>
+  </si>
+  <si>
+    <t>654321a@</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -76,14 +87,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="היפר-קישור" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -99,7 +113,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="ערכת נושא Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -394,17 +408,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07D5913E-A980-4F03-9C47-BCF4FB22C894}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A31DB94E-22FA-466C-A16B-9DE110B7CFD1}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="218" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" customWidth="1"/>
+    <col min="1" max="1" width="17.85546875" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -412,18 +426,21 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
-      <c r="B2">
-        <v>123456789</v>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{D4F327FC-0472-43CB-AD5B-87B7CF240C40}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>